<commit_message>
Improved start-stop code to allow both startup delay (with fuel usage) and Pmin>0
</commit_message>
<xml_diff>
--- a/examples/data_test2.xlsx
+++ b/examples/data_test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\OffshoreEnergySystem_OOGESO\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F643869B-88A3-45F3-8BD4-06A8B18E405F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA0A5FB-5D60-4E6F-BC65-5171FCF79F05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13872" yWindow="984" windowWidth="15708" windowHeight="12744" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="4968" yWindow="744" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1646,7 +1646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6EB10-AB47-4D11-878D-7EA50574CBA2}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1673,7 +1673,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="4">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -2199,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G54" si="0">G3-0.02</f>
+        <f t="shared" ref="G4:G51" si="0">G3-0.02</f>
         <v>0.96</v>
       </c>
     </row>
@@ -4552,7 +4552,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H54" si="1">H3-0.02</f>
+        <f t="shared" ref="H4:H51" si="1">H3-0.02</f>
         <v>0.96</v>
       </c>
     </row>
@@ -7169,6 +7169,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -7377,15 +7386,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
   <ds:schemaRefs>
@@ -7396,6 +7396,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7412,12 +7420,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>